<commit_message>
TaskBerry Gantt Chart Final
</commit_message>
<xml_diff>
--- a/TaskBerry_GanttChart.xlsx
+++ b/TaskBerry_GanttChart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Task</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Task duration</t>
+  </si>
+  <si>
+    <t>Holidays break</t>
   </si>
 </sst>
 </file>
@@ -84,7 +87,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -266,11 +269,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -285,6 +327,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,9 +448,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Chart!$A$2:$A$4</c:f>
+              <c:f>Chart!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Initial phase</c:v>
                 </c:pt>
@@ -413,6 +458,9 @@
                   <c:v>Interim phase</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Holidays break</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Final phase</c:v>
                 </c:pt>
               </c:strCache>
@@ -420,10 +468,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Chart!$B$2:$B$4</c:f>
+              <c:f>Chart!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>43801</c:v>
                 </c:pt>
@@ -431,6 +479,9 @@
                   <c:v>43808</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>43813</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>43836</c:v>
                 </c:pt>
               </c:numCache>
@@ -461,11 +512,25 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Chart!$A$2:$A$4</c:f>
+              <c:f>Chart!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Initial phase</c:v>
                 </c:pt>
@@ -473,6 +538,9 @@
                   <c:v>Interim phase</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Holidays break</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Final phase</c:v>
                 </c:pt>
               </c:strCache>
@@ -480,10 +548,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Chart!$D$2:$D$4</c:f>
+              <c:f>Chart!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -491,6 +559,9 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
@@ -1257,7 +1328,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1543,17 +1614,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1597,28 +1667,43 @@
         <v>43812</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D4" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D5" si="0">C3-B3</f>
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="15">
+        <v>43813</v>
+      </c>
+      <c r="C4" s="15">
+        <v>43835</v>
+      </c>
+      <c r="D4" s="16">
+        <f>C4-B4</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B5" s="6">
         <v>43836</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C5" s="6">
         <v>43844</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D5" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>